<commit_message>
echarts.js and  echarts.min.js add
</commit_message>
<xml_diff>
--- a/工作安排.xlsx
+++ b/工作安排.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$57</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="272">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -972,11 +972,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间过期一个月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对话管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户状态细化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>否</t>
+    <t>没有可供测试的服务号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -984,15 +1032,74 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间过期一个月</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分细节需要打磨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>symfony环境搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>symfony学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以symfony中文网为准-了解控制器路由</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://symfony.newlifeclan.com/</t>
+  </si>
+  <si>
+    <t>已记录学习笔记，参考：http://blog.csdn.net/weng_xianhu/article/details/65633371</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成复核结果的bug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优对</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1000,27 +1107,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>对话管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>优对</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>后台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户状态细化</t>
+    <t>备忘里面的新增需求--先累计一下</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1425,10 +1512,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1443,8 +1530,9 @@
     <col min="8" max="9" width="16.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="12" max="12" width="33" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1485,7 +1573,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>52</v>
       </c>
@@ -1499,10 +1587,19 @@
         <v>235</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>236</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2">
         <v>42866</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
@@ -1913,7 +2010,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>51</v>
       </c>
@@ -1927,10 +2024,25 @@
         <v>233</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>245</v>
+        <v>40</v>
       </c>
       <c r="F16" s="2">
         <v>42866</v>
+      </c>
+      <c r="G16" s="2">
+        <v>42874</v>
+      </c>
+      <c r="I16" s="2">
+        <v>42871</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
@@ -2961,45 +3073,48 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>208</v>
+        <v>263</v>
       </c>
       <c r="F49" s="2">
-        <v>42863</v>
+        <v>42873</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>223</v>
+        <v>42</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>178</v>
+        <v>266</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>224</v>
+        <v>267</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>221</v>
+        <v>260</v>
       </c>
       <c r="F50" s="2">
-        <v>42864</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+        <v>42873</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
         <v>53</v>
       </c>
@@ -3007,19 +3122,28 @@
         <v>230</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="F51" s="2">
         <v>42864</v>
       </c>
       <c r="G51" s="2">
         <v>42867</v>
+      </c>
+      <c r="I51" s="2">
+        <v>42867</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
@@ -3042,13 +3166,13 @@
         <v>42839</v>
       </c>
       <c r="J52" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="L52" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
@@ -3065,36 +3189,36 @@
         <v>141</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F53" s="2">
         <v>42837</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K53" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="L53" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>205</v>
+        <v>10</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="F54" s="2">
         <v>42863</v>
@@ -3102,35 +3226,139 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
+        <v>49</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F55" s="2">
+        <v>42864</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F55" s="2">
+      <c r="B56" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F56" s="2">
         <v>42867</v>
       </c>
+      <c r="G56" s="2">
+        <v>42874</v>
+      </c>
+      <c r="I56" s="2">
+        <v>42872</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="2">
+        <v>42872</v>
+      </c>
+      <c r="I57" s="2">
+        <v>42873</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A58" s="1">
+        <v>45</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F58" s="2">
+        <v>42863</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F59" s="2">
+        <v>42874</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L54">
+  <autoFilter ref="A1:L57">
     <filterColumn colId="4">
       <filters>
         <filter val="A"/>
         <filter val="B"/>
-        <filter val="C"/>
+        <filter val="D"/>
       </filters>
     </filterColumn>
-    <sortState ref="A2:L54">
-      <sortCondition ref="E1:E54"/>
+    <sortState ref="A49:L58">
+      <sortCondition ref="E1:E57"/>
     </sortState>
   </autoFilter>
   <sortState ref="A1:H1">

</xml_diff>